<commit_message>
Chris update to trans/TTS, increasing BAU EV adoption to align with Gov Browns EO setting course for 5 million EVs by 2030, CA EPS v1 BAU, and UC Davis ITS carbon neutrality study
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Revised variables\Transpo updates (16-May)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Revised variables\Transpo updates (19-May-2022)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1E2E7C9-9B06-4DC5-8E19-FEB7AAAEE8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25CCA9F6-74CB-41E4-9B05-CB0203C0C894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="959">
   <si>
     <t>Source:</t>
   </si>
@@ -2916,6 +2916,18 @@
   </si>
   <si>
     <t>HDV psgr</t>
+  </si>
+  <si>
+    <t>*Adjust battery electric vehicle*</t>
+  </si>
+  <si>
+    <t>* Due to different new sales levels, adjustments from the initial model release were made to hit the BAU target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values advanced one year in time initially </t>
+  </si>
+  <si>
+    <t>Then incremented as detailed in this row to hit expected BAU</t>
   </si>
 </sst>
 </file>
@@ -5322,8 +5334,8 @@
   </sheetPr>
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:AF4"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5476,126 +5488,126 @@
       </c>
       <c r="B2">
         <f>Assumptions!B59</f>
-        <v>7.1699320999999996E-2</v>
+        <v>8.6806201999999999E-2</v>
       </c>
       <c r="C2">
         <f>Assumptions!C59</f>
-        <v>7.9299499999999995E-2</v>
+        <v>9.6378142999999999E-2</v>
       </c>
       <c r="D2">
         <f>Assumptions!D59</f>
-        <v>8.6806201999999999E-2</v>
+        <v>0.10774742800000001</v>
       </c>
       <c r="E2">
         <f>Assumptions!E59</f>
-        <v>9.6378142999999999E-2</v>
+        <v>0.12311778</v>
       </c>
       <c r="F2">
         <f>Assumptions!F59</f>
-        <v>0.10774742800000001</v>
+        <v>0.12811777999999999</v>
       </c>
       <c r="G2">
         <f>Assumptions!G59</f>
-        <v>0.12311778</v>
+        <v>0.13311777999999999</v>
       </c>
       <c r="H2">
         <f>Assumptions!H59</f>
-        <v>0.12311778</v>
+        <v>0.142107188</v>
       </c>
       <c r="I2">
         <f>Assumptions!I59</f>
-        <v>0.12311778</v>
+        <v>0.16099779</v>
       </c>
       <c r="J2">
         <f>Assumptions!J59</f>
-        <v>0.12710718800000001</v>
+        <v>0.18444923299999999</v>
       </c>
       <c r="K2">
         <f>Assumptions!K59</f>
-        <v>0.14099779000000001</v>
+        <v>0.22931154200000001</v>
       </c>
       <c r="L2">
         <f>Assumptions!L59</f>
-        <v>0.159449233</v>
+        <v>0.27915663899999998</v>
       </c>
       <c r="M2">
         <f>Assumptions!M59</f>
-        <v>0.19931154200000001</v>
+        <v>0.293598358</v>
       </c>
       <c r="N2">
         <f>Assumptions!N59</f>
-        <v>0.24415663900000001</v>
+        <v>0.34710665899999998</v>
       </c>
       <c r="O2">
         <f>Assumptions!O59</f>
-        <v>0.293598358</v>
+        <v>0.40404082800000002</v>
       </c>
       <c r="P2">
         <f>Assumptions!P59</f>
-        <v>0.34710665899999998</v>
+        <v>0.463686345</v>
       </c>
       <c r="Q2">
         <f>Assumptions!Q59</f>
-        <v>0.40404082800000002</v>
+        <v>0.52529182900000004</v>
       </c>
       <c r="R2">
         <f>Assumptions!R59</f>
-        <v>0.463686345</v>
+        <v>0.58810319300000002</v>
       </c>
       <c r="S2">
         <f>Assumptions!S59</f>
-        <v>0.52529182900000004</v>
+        <v>0.65139297799999996</v>
       </c>
       <c r="T2">
         <f>Assumptions!T59</f>
-        <v>0.58810319300000002</v>
+        <v>0.71448372400000004</v>
       </c>
       <c r="U2">
         <f>Assumptions!U59</f>
-        <v>0.65139297799999996</v>
+        <v>0.77676499200000004</v>
       </c>
       <c r="V2">
         <f>Assumptions!V59</f>
-        <v>0.71448372400000004</v>
+        <v>0.837704263</v>
       </c>
       <c r="W2">
         <f>Assumptions!W59</f>
-        <v>0.77676499200000004</v>
+        <v>0.89685236999999995</v>
       </c>
       <c r="X2">
         <f>Assumptions!X59</f>
-        <v>0.837704263</v>
+        <v>0.95384432900000005</v>
       </c>
       <c r="Y2">
         <f>Assumptions!Y59</f>
-        <v>0.89685236999999995</v>
+        <v>1</v>
       </c>
       <c r="Z2">
         <f>Assumptions!Z59</f>
-        <v>0.95384432900000005</v>
+        <v>1</v>
       </c>
       <c r="AA2">
         <f>Assumptions!AA59</f>
         <v>1</v>
       </c>
       <c r="AB2">
-        <f>Assumptions!AB59</f>
+        <f>Assumptions!Z60</f>
         <v>1</v>
       </c>
       <c r="AC2">
-        <f>Assumptions!AC59</f>
+        <f>Assumptions!AA60</f>
         <v>1</v>
       </c>
       <c r="AD2">
-        <f>Assumptions!AD59</f>
+        <f>Assumptions!AB60</f>
         <v>1</v>
       </c>
       <c r="AE2">
-        <f>Assumptions!AE59</f>
+        <f>Assumptions!AC60</f>
         <v>1</v>
       </c>
       <c r="AF2">
-        <f>Assumptions!AF59</f>
+        <f>Assumptions!AD60</f>
         <v>1</v>
       </c>
     </row>
@@ -5960,127 +5972,127 @@
         <v>5</v>
       </c>
       <c r="B6" s="15">
-        <f>Assumptions!B63</f>
+        <f>Assumptions!B64</f>
         <v>1.9460552999999998E-2</v>
       </c>
       <c r="C6" s="15">
-        <f>Assumptions!C63</f>
+        <f>Assumptions!C64</f>
         <v>2.0337040000000001E-2</v>
       </c>
       <c r="D6" s="15">
-        <f>Assumptions!D63</f>
+        <f>Assumptions!D64</f>
         <v>2.0885547000000001E-2</v>
       </c>
       <c r="E6" s="15">
-        <f>Assumptions!E63</f>
+        <f>Assumptions!E64</f>
         <v>2.1811047E-2</v>
       </c>
       <c r="F6" s="15">
-        <f>Assumptions!F63</f>
+        <f>Assumptions!F64</f>
         <v>2.2789772E-2</v>
       </c>
       <c r="G6" s="15">
-        <f>Assumptions!G63</f>
+        <f>Assumptions!G64</f>
         <v>2.4530158E-2</v>
       </c>
       <c r="H6" s="15">
-        <f>Assumptions!H63</f>
+        <f>Assumptions!H64</f>
         <v>1.9105086E-2</v>
       </c>
       <c r="I6" s="15">
-        <f>Assumptions!I63</f>
+        <f>Assumptions!I64</f>
         <v>2.5750637E-2</v>
       </c>
       <c r="J6" s="15">
-        <f>Assumptions!J63</f>
+        <f>Assumptions!J64</f>
         <v>2.9856924999999999E-2</v>
       </c>
       <c r="K6" s="15">
-        <f>Assumptions!K63</f>
+        <f>Assumptions!K64</f>
         <v>3.3546773000000002E-2</v>
       </c>
       <c r="L6" s="15">
-        <f>Assumptions!L63</f>
+        <f>Assumptions!L64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="M6" s="15">
-        <f>Assumptions!M63</f>
+        <f>Assumptions!M64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="N6" s="15">
-        <f>Assumptions!N63</f>
+        <f>Assumptions!N64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="O6" s="15">
-        <f>Assumptions!O63</f>
+        <f>Assumptions!O64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="P6" s="15">
-        <f>Assumptions!P63</f>
+        <f>Assumptions!P64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="Q6" s="15">
-        <f>Assumptions!Q63</f>
+        <f>Assumptions!Q64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="R6" s="15">
-        <f>Assumptions!R63</f>
+        <f>Assumptions!R64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="S6" s="15">
-        <f>Assumptions!S63</f>
+        <f>Assumptions!S64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="T6" s="15">
-        <f>Assumptions!T63</f>
+        <f>Assumptions!T64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="U6" s="15">
-        <f>Assumptions!U63</f>
+        <f>Assumptions!U64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="V6" s="15">
-        <f>Assumptions!V63</f>
+        <f>Assumptions!V64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="W6" s="15">
-        <f>Assumptions!W63</f>
+        <f>Assumptions!W64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="X6" s="15">
-        <f>Assumptions!X63</f>
+        <f>Assumptions!X64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="Y6" s="15">
-        <f>Assumptions!Y63</f>
+        <f>Assumptions!Y64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="Z6" s="15">
-        <f>Assumptions!Z63</f>
+        <f>Assumptions!Z64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="AA6" s="15">
-        <f>Assumptions!AA63</f>
+        <f>Assumptions!AA64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="AB6" s="15">
-        <f>Assumptions!AB63</f>
+        <f>Assumptions!AB64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="AC6" s="15">
-        <f>Assumptions!AC63</f>
+        <f>Assumptions!AC64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="AD6" s="15">
-        <f>Assumptions!AD63</f>
+        <f>Assumptions!AD64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="AE6" s="15">
-        <f>Assumptions!AE63</f>
+        <f>Assumptions!AE64</f>
         <v>3.7123840999999998E-2</v>
       </c>
       <c r="AF6" s="15">
-        <f>Assumptions!AF63</f>
+        <f>Assumptions!AF64</f>
         <v>3.7123840999999998E-2</v>
       </c>
     </row>
@@ -6468,127 +6480,127 @@
         <v>1</v>
       </c>
       <c r="B2" s="15">
-        <f>Assumptions!B69</f>
+        <f>Assumptions!B74</f>
         <v>4.0288390000000002E-3</v>
       </c>
       <c r="C2" s="15">
-        <f>Assumptions!C69</f>
+        <f>Assumptions!C74</f>
         <v>7.4906770000000003E-3</v>
       </c>
       <c r="D2" s="15">
-        <f>Assumptions!D69</f>
+        <f>Assumptions!D74</f>
         <v>1.3517357000000001E-2</v>
       </c>
       <c r="E2" s="15">
-        <f>Assumptions!E69</f>
+        <f>Assumptions!E74</f>
         <v>2.2982546E-2</v>
       </c>
       <c r="F2" s="15">
-        <f>Assumptions!F69</f>
+        <f>Assumptions!F74</f>
         <v>3.6100624999999997E-2</v>
       </c>
       <c r="G2" s="15">
-        <f>Assumptions!G69</f>
+        <f>Assumptions!G74</f>
         <v>5.1007505000000002E-2</v>
       </c>
       <c r="H2" s="15">
-        <f>Assumptions!H69</f>
+        <f>Assumptions!H74</f>
         <v>6.5037979999999995E-2</v>
       </c>
       <c r="I2" s="15">
-        <f>Assumptions!I69</f>
+        <f>Assumptions!I74</f>
         <v>7.4050884999999997E-2</v>
       </c>
       <c r="J2" s="15">
-        <f>Assumptions!J69</f>
+        <f>Assumptions!J74</f>
         <v>7.5902622000000003E-2</v>
       </c>
       <c r="K2" s="15">
-        <f>Assumptions!K69</f>
+        <f>Assumptions!K74</f>
         <v>7.9969093000000005E-2</v>
       </c>
       <c r="L2" s="15">
-        <f>Assumptions!L69</f>
+        <f>Assumptions!L74</f>
         <v>8.5852278000000004E-2</v>
       </c>
       <c r="M2" s="15">
-        <f>Assumptions!M69</f>
+        <f>Assumptions!M74</f>
         <v>0.115342836</v>
       </c>
       <c r="N2" s="15">
-        <f>Assumptions!N69</f>
+        <f>Assumptions!N74</f>
         <v>0.12811123299999999</v>
       </c>
       <c r="O2" s="15">
-        <f>Assumptions!O69</f>
+        <f>Assumptions!O74</f>
         <v>0.14218904299999999</v>
       </c>
       <c r="P2" s="15">
-        <f>Assumptions!P69</f>
+        <f>Assumptions!P74</f>
         <v>0.15715570200000001</v>
       </c>
       <c r="Q2" s="15">
-        <f>Assumptions!Q69</f>
+        <f>Assumptions!Q74</f>
         <v>0.17312130100000001</v>
       </c>
       <c r="R2" s="15">
-        <f>Assumptions!R69</f>
+        <f>Assumptions!R74</f>
         <v>0.18486860099999999</v>
       </c>
       <c r="S2" s="15">
-        <f>Assumptions!S69</f>
+        <f>Assumptions!S74</f>
         <v>0.194230549</v>
       </c>
       <c r="T2" s="15">
-        <f>Assumptions!T69</f>
+        <f>Assumptions!T74</f>
         <v>0.200844037</v>
       </c>
       <c r="U2" s="15">
-        <f>Assumptions!U69</f>
+        <f>Assumptions!U74</f>
         <v>0.20479752200000001</v>
       </c>
       <c r="V2" s="15">
-        <f>Assumptions!V69</f>
+        <f>Assumptions!V74</f>
         <v>0.20639531</v>
       </c>
       <c r="W2" s="15">
-        <f>Assumptions!W69</f>
+        <f>Assumptions!W74</f>
         <v>0.207285109</v>
       </c>
       <c r="X2" s="15">
-        <f>Assumptions!X69</f>
+        <f>Assumptions!X74</f>
         <v>0.205884558</v>
       </c>
       <c r="Y2" s="15">
-        <f>Assumptions!Y69</f>
+        <f>Assumptions!Y74</f>
         <v>0.203850332</v>
       </c>
       <c r="Z2" s="15">
-        <f>Assumptions!Z69</f>
+        <f>Assumptions!Z74</f>
         <v>0.20227350999999999</v>
       </c>
       <c r="AA2" s="15">
-        <f>Assumptions!AA69</f>
+        <f>Assumptions!AA74</f>
         <v>0.201661221</v>
       </c>
       <c r="AB2" s="15">
-        <f>Assumptions!AB69</f>
+        <f>Assumptions!AB74</f>
         <v>0.202610965</v>
       </c>
       <c r="AC2" s="15">
-        <f>Assumptions!AC69</f>
+        <f>Assumptions!AC74</f>
         <v>0.20489760400000001</v>
       </c>
       <c r="AD2" s="15">
-        <f>Assumptions!AD69</f>
+        <f>Assumptions!AD74</f>
         <v>0.20845095499999999</v>
       </c>
       <c r="AE2" s="15">
-        <f>Assumptions!AE69</f>
+        <f>Assumptions!AE74</f>
         <v>0.21348747400000001</v>
       </c>
       <c r="AF2" s="15">
-        <f>Assumptions!AF69</f>
+        <f>Assumptions!AF74</f>
         <v>0.22004099999999999</v>
       </c>
     </row>
@@ -7378,7 +7390,7 @@
   </sheetPr>
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AF8"/>
     </sheetView>
   </sheetViews>
@@ -7522,127 +7534,127 @@
         <v>1</v>
       </c>
       <c r="B2" s="15">
-        <f>Assumptions!B89</f>
+        <f>Assumptions!B94</f>
         <v>3.8708444000000002E-2</v>
       </c>
       <c r="C2" s="15">
-        <f>Assumptions!C89</f>
+        <f>Assumptions!C94</f>
         <v>4.6440683000000003E-2</v>
       </c>
       <c r="D2" s="15">
-        <f>Assumptions!D89</f>
+        <f>Assumptions!D94</f>
         <v>5.4172921999999998E-2</v>
       </c>
       <c r="E2" s="15">
-        <f>Assumptions!E89</f>
+        <f>Assumptions!E94</f>
         <v>6.1905160000000001E-2</v>
       </c>
       <c r="F2" s="15">
-        <f>Assumptions!F89</f>
+        <f>Assumptions!F94</f>
         <v>6.9637399000000003E-2</v>
       </c>
       <c r="G2" s="15">
-        <f>Assumptions!G89</f>
+        <f>Assumptions!G94</f>
         <v>7.7369637000000005E-2</v>
       </c>
       <c r="H2" s="15">
-        <f>Assumptions!H89</f>
+        <f>Assumptions!H94</f>
         <v>8.5101876000000007E-2</v>
       </c>
       <c r="I2" s="15">
-        <f>Assumptions!I89</f>
+        <f>Assumptions!I94</f>
         <v>9.2834114999999995E-2</v>
       </c>
       <c r="J2" s="15">
-        <f>Assumptions!J89</f>
+        <f>Assumptions!J94</f>
         <v>0.100566353</v>
       </c>
       <c r="K2" s="15">
-        <f>Assumptions!K89</f>
+        <f>Assumptions!K94</f>
         <v>0.108298592</v>
       </c>
       <c r="L2" s="15">
-        <f>Assumptions!L89</f>
+        <f>Assumptions!L94</f>
         <v>0.11603083</v>
       </c>
       <c r="M2" s="15">
-        <f>Assumptions!M89</f>
+        <f>Assumptions!M94</f>
         <v>0.123763069</v>
       </c>
       <c r="N2" s="15">
-        <f>Assumptions!N89</f>
+        <f>Assumptions!N94</f>
         <v>0.13149530700000001</v>
       </c>
       <c r="O2" s="15">
-        <f>Assumptions!O89</f>
+        <f>Assumptions!O94</f>
         <v>0.13922754600000001</v>
       </c>
       <c r="P2" s="15">
-        <f>Assumptions!P89</f>
+        <f>Assumptions!P94</f>
         <v>0.14695978500000001</v>
       </c>
       <c r="Q2" s="15">
-        <f>Assumptions!Q89</f>
+        <f>Assumptions!Q94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="R2" s="15">
-        <f>Assumptions!R89</f>
+        <f>Assumptions!R94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="S2" s="15">
-        <f>Assumptions!S89</f>
+        <f>Assumptions!S94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="T2" s="15">
-        <f>Assumptions!T89</f>
+        <f>Assumptions!T94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="U2" s="15">
-        <f>Assumptions!U89</f>
+        <f>Assumptions!U94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="V2" s="15">
-        <f>Assumptions!V89</f>
+        <f>Assumptions!V94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="W2" s="15">
-        <f>Assumptions!W89</f>
+        <f>Assumptions!W94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="X2" s="15">
-        <f>Assumptions!X89</f>
+        <f>Assumptions!X94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="Y2" s="15">
-        <f>Assumptions!Y89</f>
+        <f>Assumptions!Y94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="Z2" s="15">
-        <f>Assumptions!Z89</f>
+        <f>Assumptions!Z94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="AA2" s="15">
-        <f>Assumptions!AA89</f>
+        <f>Assumptions!AA94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="AB2" s="15">
-        <f>Assumptions!AB89</f>
+        <f>Assumptions!AB94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="AC2" s="15">
-        <f>Assumptions!AC89</f>
+        <f>Assumptions!AC94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="AD2" s="15">
-        <f>Assumptions!AD89</f>
+        <f>Assumptions!AD94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="AE2" s="15">
-        <f>Assumptions!AE89</f>
+        <f>Assumptions!AE94</f>
         <v>0.16242426200000001</v>
       </c>
       <c r="AF2" s="15">
-        <f>Assumptions!AF89</f>
+        <f>Assumptions!AF94</f>
         <v>0.16242426200000001</v>
       </c>
     </row>
@@ -8576,127 +8588,127 @@
         <v>1</v>
       </c>
       <c r="B2" s="15">
-        <f>Assumptions!B79</f>
+        <f>Assumptions!B84</f>
         <v>2.162813E-3</v>
       </c>
       <c r="C2" s="15">
-        <f>Assumptions!C79</f>
+        <f>Assumptions!C84</f>
         <v>2.3154429999999999E-3</v>
       </c>
       <c r="D2" s="15">
-        <f>Assumptions!D79</f>
+        <f>Assumptions!D84</f>
         <v>3.8036620000000002E-3</v>
       </c>
       <c r="E2" s="15">
-        <f>Assumptions!E79</f>
+        <f>Assumptions!E84</f>
         <v>5.3024580000000003E-3</v>
       </c>
       <c r="F2" s="15">
-        <f>Assumptions!F79</f>
+        <f>Assumptions!F84</f>
         <v>6.8161840000000003E-3</v>
       </c>
       <c r="G2" s="15">
-        <f>Assumptions!G79</f>
+        <f>Assumptions!G84</f>
         <v>8.3520650000000005E-3</v>
       </c>
       <c r="H2" s="15">
-        <f>Assumptions!H79</f>
+        <f>Assumptions!H84</f>
         <v>9.9196909999999996E-3</v>
       </c>
       <c r="I2" s="15">
-        <f>Assumptions!I79</f>
+        <f>Assumptions!I84</f>
         <v>1.1533804E-2</v>
       </c>
       <c r="J2" s="15">
-        <f>Assumptions!J79</f>
+        <f>Assumptions!J84</f>
         <v>1.3212750000000001E-2</v>
       </c>
       <c r="K2" s="15">
-        <f>Assumptions!K79</f>
+        <f>Assumptions!K84</f>
         <v>1.4978709E-2</v>
       </c>
       <c r="L2" s="15">
-        <f>Assumptions!L79</f>
+        <f>Assumptions!L84</f>
         <v>1.6867157000000001E-2</v>
       </c>
       <c r="M2" s="15">
-        <f>Assumptions!M79</f>
+        <f>Assumptions!M84</f>
         <v>1.7452430000000001E-2</v>
       </c>
       <c r="N2" s="15">
-        <f>Assumptions!N79</f>
+        <f>Assumptions!N84</f>
         <v>1.8252092000000001E-2</v>
       </c>
       <c r="O2" s="15">
-        <f>Assumptions!O79</f>
+        <f>Assumptions!O84</f>
         <v>1.9309627999999999E-2</v>
       </c>
       <c r="P2" s="15">
-        <f>Assumptions!P79</f>
+        <f>Assumptions!P84</f>
         <v>2.0645547E-2</v>
       </c>
       <c r="Q2" s="15">
-        <f>Assumptions!Q79</f>
+        <f>Assumptions!Q84</f>
         <v>2.227985E-2</v>
       </c>
       <c r="R2" s="15">
-        <f>Assumptions!R79</f>
+        <f>Assumptions!R84</f>
         <v>2.4351382000000001E-2</v>
       </c>
       <c r="S2" s="15">
-        <f>Assumptions!S79</f>
+        <f>Assumptions!S84</f>
         <v>2.6780347999999999E-2</v>
       </c>
       <c r="T2" s="15">
-        <f>Assumptions!T79</f>
+        <f>Assumptions!T84</f>
         <v>2.9592798E-2</v>
       </c>
       <c r="U2" s="15">
-        <f>Assumptions!U79</f>
+        <f>Assumptions!U84</f>
         <v>3.2960165999999999E-2</v>
       </c>
       <c r="V2" s="15">
-        <f>Assumptions!V79</f>
+        <f>Assumptions!V84</f>
         <v>3.7044072999999997E-2</v>
       </c>
       <c r="W2" s="15">
-        <f>Assumptions!W79</f>
+        <f>Assumptions!W84</f>
         <v>4.2587001999999999E-2</v>
       </c>
       <c r="X2" s="15">
-        <f>Assumptions!X79</f>
+        <f>Assumptions!X84</f>
         <v>4.8824688999999998E-2</v>
       </c>
       <c r="Y2" s="15">
-        <f>Assumptions!Y79</f>
+        <f>Assumptions!Y84</f>
         <v>5.5696411000000001E-2</v>
       </c>
       <c r="Z2" s="15">
-        <f>Assumptions!Z79</f>
+        <f>Assumptions!Z84</f>
         <v>6.2507718000000004E-2</v>
       </c>
       <c r="AA2" s="15">
-        <f>Assumptions!AA79</f>
+        <f>Assumptions!AA84</f>
         <v>6.8291605000000005E-2</v>
       </c>
       <c r="AB2" s="15">
-        <f>Assumptions!AB79</f>
+        <f>Assumptions!AB84</f>
         <v>7.2692810999999996E-2</v>
       </c>
       <c r="AC2" s="15">
-        <f>Assumptions!AC79</f>
+        <f>Assumptions!AC84</f>
         <v>7.5988175000000005E-2</v>
       </c>
       <c r="AD2" s="15">
-        <f>Assumptions!AD79</f>
+        <f>Assumptions!AD84</f>
         <v>7.8326194000000002E-2</v>
       </c>
       <c r="AE2" s="15">
-        <f>Assumptions!AE79</f>
+        <f>Assumptions!AE84</f>
         <v>8.0239419000000006E-2</v>
       </c>
       <c r="AF2" s="15">
-        <f>Assumptions!AF79</f>
+        <f>Assumptions!AF84</f>
         <v>8.1928860000000006E-2</v>
       </c>
     </row>
@@ -54458,10 +54470,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AF89"/>
+  <dimension ref="A1:AF94"/>
   <sheetViews>
-    <sheetView topLeftCell="R71" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89:AF89"/>
+    <sheetView topLeftCell="P57" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:AA59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54771,2373 +54783,2538 @@
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
+        <v>955</v>
+      </c>
+      <c r="B59" s="15">
+        <f t="shared" ref="B59:G59" si="0">B60</f>
+        <v>8.6806201999999999E-2</v>
+      </c>
+      <c r="C59" s="15">
+        <f t="shared" si="0"/>
+        <v>9.6378142999999999E-2</v>
+      </c>
+      <c r="D59" s="15">
+        <f t="shared" si="0"/>
+        <v>0.10774742800000001</v>
+      </c>
+      <c r="E59" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12311778</v>
+      </c>
+      <c r="F59" s="15">
+        <f>F60+F70</f>
+        <v>0.12811777999999999</v>
+      </c>
+      <c r="G59" s="15">
+        <f t="shared" ref="G59:L59" si="1">G60+G70</f>
+        <v>0.13311777999999999</v>
+      </c>
+      <c r="H59" s="15">
+        <f t="shared" si="1"/>
+        <v>0.142107188</v>
+      </c>
+      <c r="I59" s="15">
+        <f t="shared" si="1"/>
+        <v>0.16099779</v>
+      </c>
+      <c r="J59" s="15">
+        <f t="shared" si="1"/>
+        <v>0.18444923299999999</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="1"/>
+        <v>0.22931154200000001</v>
+      </c>
+      <c r="L59" s="15">
+        <f t="shared" si="1"/>
+        <v>0.27915663899999998</v>
+      </c>
+      <c r="M59" s="15">
+        <f>M60</f>
+        <v>0.293598358</v>
+      </c>
+      <c r="N59" s="15">
+        <f t="shared" ref="N59:AA59" si="2">N60</f>
+        <v>0.34710665899999998</v>
+      </c>
+      <c r="O59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.40404082800000002</v>
+      </c>
+      <c r="P59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.463686345</v>
+      </c>
+      <c r="Q59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.52529182900000004</v>
+      </c>
+      <c r="R59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.58810319300000002</v>
+      </c>
+      <c r="S59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.65139297799999996</v>
+      </c>
+      <c r="T59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.71448372400000004</v>
+      </c>
+      <c r="U59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.77676499200000004</v>
+      </c>
+      <c r="V59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.837704263</v>
+      </c>
+      <c r="W59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.89685236999999995</v>
+      </c>
+      <c r="X59" s="15">
+        <f t="shared" si="2"/>
+        <v>0.95384432900000005</v>
+      </c>
+      <c r="Y59" s="15">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="B59" s="15">
-        <v>7.1699320999999996E-2</v>
-      </c>
-      <c r="C59" s="15">
-        <v>7.9299499999999995E-2</v>
-      </c>
-      <c r="D59" s="15">
-        <v>8.6806201999999999E-2</v>
-      </c>
-      <c r="E59" s="15">
-        <v>9.6378142999999999E-2</v>
-      </c>
-      <c r="F59" s="15">
-        <v>0.10774742800000001</v>
-      </c>
-      <c r="G59" s="15">
-        <v>0.12311778</v>
-      </c>
-      <c r="H59" s="15">
-        <v>0.12311778</v>
-      </c>
-      <c r="I59" s="15">
-        <v>0.12311778</v>
-      </c>
-      <c r="J59" s="15">
-        <v>0.12710718800000001</v>
-      </c>
-      <c r="K59" s="15">
-        <v>0.14099779000000001</v>
-      </c>
-      <c r="L59" s="15">
-        <v>0.159449233</v>
-      </c>
-      <c r="M59" s="15">
-        <v>0.19931154200000001</v>
-      </c>
-      <c r="N59" s="15">
-        <v>0.24415663900000001</v>
-      </c>
-      <c r="O59" s="15">
-        <v>0.293598358</v>
-      </c>
-      <c r="P59" s="15">
-        <v>0.34710665899999998</v>
-      </c>
-      <c r="Q59" s="15">
-        <v>0.40404082800000002</v>
-      </c>
-      <c r="R59" s="15">
-        <v>0.463686345</v>
-      </c>
-      <c r="S59" s="15">
-        <v>0.52529182900000004</v>
-      </c>
-      <c r="T59" s="15">
-        <v>0.58810319300000002</v>
-      </c>
-      <c r="U59" s="15">
-        <v>0.65139297799999996</v>
-      </c>
-      <c r="V59" s="15">
-        <v>0.71448372400000004</v>
-      </c>
-      <c r="W59" s="15">
-        <v>0.77676499200000004</v>
-      </c>
-      <c r="X59" s="15">
-        <v>0.837704263</v>
-      </c>
-      <c r="Y59" s="15">
-        <v>0.89685236999999995</v>
-      </c>
       <c r="Z59" s="15">
-        <v>0.95384432900000005</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="AA59" s="15">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AB59" s="15">
+        <f t="shared" ref="AB59:AF59" si="3">Z60</f>
         <v>1</v>
       </c>
       <c r="AC59" s="15">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AD59" s="15">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE59" s="15">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AF59" s="15">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A60" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" s="15">
-        <v>0</v>
+        <v>8.6806201999999999E-2</v>
       </c>
       <c r="C60" s="15">
-        <v>0</v>
+        <v>9.6378142999999999E-2</v>
       </c>
       <c r="D60" s="15">
-        <v>0</v>
+        <v>0.10774742800000001</v>
       </c>
       <c r="E60" s="15">
-        <v>0</v>
+        <v>0.12311778</v>
       </c>
       <c r="F60" s="15">
-        <v>0</v>
+        <v>0.12311778</v>
       </c>
       <c r="G60" s="15">
-        <v>0</v>
+        <v>0.12311778</v>
       </c>
       <c r="H60" s="15">
-        <v>0</v>
+        <v>0.12710718800000001</v>
       </c>
       <c r="I60" s="15">
-        <v>0</v>
+        <v>0.14099779000000001</v>
       </c>
       <c r="J60" s="15">
-        <v>0</v>
+        <v>0.159449233</v>
       </c>
       <c r="K60" s="15">
-        <v>0</v>
+        <v>0.19931154200000001</v>
       </c>
       <c r="L60" s="15">
-        <v>0</v>
+        <v>0.24415663900000001</v>
       </c>
       <c r="M60" s="15">
-        <v>0</v>
+        <v>0.293598358</v>
       </c>
       <c r="N60" s="15">
-        <v>0</v>
+        <v>0.34710665899999998</v>
       </c>
       <c r="O60" s="15">
-        <v>0</v>
+        <v>0.40404082800000002</v>
       </c>
       <c r="P60" s="15">
-        <v>0</v>
+        <v>0.463686345</v>
       </c>
       <c r="Q60" s="15">
-        <v>0</v>
+        <v>0.52529182900000004</v>
       </c>
       <c r="R60" s="15">
-        <v>0</v>
+        <v>0.58810319300000002</v>
       </c>
       <c r="S60" s="15">
-        <v>0</v>
+        <v>0.65139297799999996</v>
       </c>
       <c r="T60" s="15">
-        <v>0</v>
+        <v>0.71448372400000004</v>
       </c>
       <c r="U60" s="15">
-        <v>0</v>
+        <v>0.77676499200000004</v>
       </c>
       <c r="V60" s="15">
-        <v>0</v>
+        <v>0.837704263</v>
       </c>
       <c r="W60" s="15">
-        <v>0</v>
+        <v>0.89685236999999995</v>
       </c>
       <c r="X60" s="15">
-        <v>0</v>
+        <v>0.95384432900000005</v>
       </c>
       <c r="Y60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD60" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE60" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A62" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63" s="15">
-        <v>1.9460552999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="C63" s="15">
-        <v>2.0337040000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D63" s="15">
-        <v>2.0885547000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E63" s="15">
-        <v>2.1811047E-2</v>
+        <v>0</v>
       </c>
       <c r="F63" s="15">
-        <v>2.2789772E-2</v>
+        <v>0</v>
       </c>
       <c r="G63" s="15">
-        <v>2.4530158E-2</v>
+        <v>0</v>
       </c>
       <c r="H63" s="15">
-        <v>1.9105086E-2</v>
+        <v>0</v>
       </c>
       <c r="I63" s="15">
-        <v>2.5750637E-2</v>
+        <v>0</v>
       </c>
       <c r="J63" s="15">
-        <v>2.9856924999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="K63" s="15">
-        <v>3.3546773000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="L63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="M63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="N63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="O63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="P63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Q63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="R63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="S63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="T63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="U63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="V63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="W63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="X63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Y63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Z63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AA63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AB63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AC63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AD63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AE63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AF63" s="15">
-        <v>3.7123840999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A64" s="15" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B64" s="15">
-        <v>0</v>
+        <v>1.9460552999999998E-2</v>
       </c>
       <c r="C64" s="15">
-        <v>0</v>
+        <v>2.0337040000000001E-2</v>
       </c>
       <c r="D64" s="15">
-        <v>0</v>
+        <v>2.0885547000000001E-2</v>
       </c>
       <c r="E64" s="15">
-        <v>0</v>
+        <v>2.1811047E-2</v>
       </c>
       <c r="F64" s="15">
-        <v>0</v>
+        <v>2.2789772E-2</v>
       </c>
       <c r="G64" s="15">
-        <v>0</v>
+        <v>2.4530158E-2</v>
       </c>
       <c r="H64" s="15">
-        <v>0</v>
+        <v>1.9105086E-2</v>
       </c>
       <c r="I64" s="15">
-        <v>0</v>
+        <v>2.5750637E-2</v>
       </c>
       <c r="J64" s="15">
-        <v>0</v>
+        <v>2.9856924999999999E-2</v>
       </c>
       <c r="K64" s="15">
-        <v>0</v>
+        <v>3.3546773000000002E-2</v>
       </c>
       <c r="L64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="M64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="N64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="O64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="P64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="Q64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="R64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="S64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="T64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="U64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="V64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="W64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="X64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="Y64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="Z64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="AA64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="AB64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="AC64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="AD64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="AE64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
       <c r="AF64" s="15">
-        <v>0</v>
+        <v>3.7123840999999998E-2</v>
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A65" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="15">
+        <v>0</v>
+      </c>
+      <c r="C65" s="15">
+        <v>0</v>
+      </c>
+      <c r="D65" s="15">
+        <v>0</v>
+      </c>
+      <c r="E65" s="15">
+        <v>0</v>
+      </c>
+      <c r="F65" s="15">
+        <v>0</v>
+      </c>
+      <c r="G65" s="15">
+        <v>0</v>
+      </c>
+      <c r="H65" s="15">
+        <v>0</v>
+      </c>
+      <c r="I65" s="15">
+        <v>0</v>
+      </c>
+      <c r="J65" s="15">
+        <v>0</v>
+      </c>
+      <c r="K65" s="15">
+        <v>0</v>
+      </c>
+      <c r="L65" s="15">
+        <v>0</v>
+      </c>
+      <c r="M65" s="15">
+        <v>0</v>
+      </c>
+      <c r="N65" s="15">
+        <v>0</v>
+      </c>
+      <c r="O65" s="15">
+        <v>0</v>
+      </c>
+      <c r="P65" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="15">
+        <v>0</v>
+      </c>
+      <c r="R65" s="15">
+        <v>0</v>
+      </c>
+      <c r="S65" s="15">
+        <v>0</v>
+      </c>
+      <c r="T65" s="15">
+        <v>0</v>
+      </c>
+      <c r="U65" s="15">
+        <v>0</v>
+      </c>
+      <c r="V65" s="15">
+        <v>0</v>
+      </c>
+      <c r="W65" s="15">
+        <v>0</v>
+      </c>
+      <c r="X65" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A66" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="15">
-        <v>0</v>
-      </c>
-      <c r="C65" s="15">
-        <v>0</v>
-      </c>
-      <c r="D65" s="15">
-        <v>0</v>
-      </c>
-      <c r="E65" s="15">
-        <v>0</v>
-      </c>
-      <c r="F65" s="15">
-        <v>0</v>
-      </c>
-      <c r="G65" s="15">
-        <v>0</v>
-      </c>
-      <c r="H65" s="15">
-        <v>0</v>
-      </c>
-      <c r="I65" s="15">
-        <v>0</v>
-      </c>
-      <c r="J65" s="15">
-        <v>0</v>
-      </c>
-      <c r="K65" s="15">
-        <v>0</v>
-      </c>
-      <c r="L65" s="15">
-        <v>0</v>
-      </c>
-      <c r="M65" s="15">
-        <v>0</v>
-      </c>
-      <c r="N65" s="15">
-        <v>0</v>
-      </c>
-      <c r="O65" s="15">
-        <v>0</v>
-      </c>
-      <c r="P65" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="15">
-        <v>0</v>
-      </c>
-      <c r="R65" s="15">
-        <v>0</v>
-      </c>
-      <c r="S65" s="15">
-        <v>0</v>
-      </c>
-      <c r="T65" s="15">
-        <v>0</v>
-      </c>
-      <c r="U65" s="15">
-        <v>0</v>
-      </c>
-      <c r="V65" s="15">
-        <v>0</v>
-      </c>
-      <c r="W65" s="15">
-        <v>0</v>
-      </c>
-      <c r="X65" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA65" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB65" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC65" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD65" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE65" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF65" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A67" s="14" t="s">
-        <v>952</v>
+      <c r="B66" s="15">
+        <v>0</v>
+      </c>
+      <c r="C66" s="15">
+        <v>0</v>
+      </c>
+      <c r="D66" s="15">
+        <v>0</v>
+      </c>
+      <c r="E66" s="15">
+        <v>0</v>
+      </c>
+      <c r="F66" s="15">
+        <v>0</v>
+      </c>
+      <c r="G66" s="15">
+        <v>0</v>
+      </c>
+      <c r="H66" s="15">
+        <v>0</v>
+      </c>
+      <c r="I66" s="15">
+        <v>0</v>
+      </c>
+      <c r="J66" s="15">
+        <v>0</v>
+      </c>
+      <c r="K66" s="15">
+        <v>0</v>
+      </c>
+      <c r="L66" s="15">
+        <v>0</v>
+      </c>
+      <c r="M66" s="15">
+        <v>0</v>
+      </c>
+      <c r="N66" s="15">
+        <v>0</v>
+      </c>
+      <c r="O66" s="15">
+        <v>0</v>
+      </c>
+      <c r="P66" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="15">
+        <v>0</v>
+      </c>
+      <c r="R66" s="15">
+        <v>0</v>
+      </c>
+      <c r="S66" s="15">
+        <v>0</v>
+      </c>
+      <c r="T66" s="15">
+        <v>0</v>
+      </c>
+      <c r="U66" s="15">
+        <v>0</v>
+      </c>
+      <c r="V66" s="15">
+        <v>0</v>
+      </c>
+      <c r="W66" s="15">
+        <v>0</v>
+      </c>
+      <c r="X66" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE66" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF66" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A68" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" s="15">
-        <v>2020</v>
-      </c>
-      <c r="C68" s="15">
-        <v>2021</v>
-      </c>
-      <c r="D68" s="15">
-        <v>2022</v>
-      </c>
-      <c r="E68" s="15">
-        <v>2023</v>
-      </c>
-      <c r="F68" s="15">
-        <v>2024</v>
-      </c>
-      <c r="G68" s="15">
-        <v>2025</v>
-      </c>
-      <c r="H68" s="15">
-        <v>2026</v>
-      </c>
-      <c r="I68" s="15">
-        <v>2027</v>
-      </c>
-      <c r="J68" s="15">
-        <v>2028</v>
-      </c>
-      <c r="K68" s="15">
-        <v>2029</v>
-      </c>
-      <c r="L68" s="15">
-        <v>2030</v>
-      </c>
-      <c r="M68" s="15">
-        <v>2031</v>
-      </c>
-      <c r="N68" s="15">
-        <v>2032</v>
-      </c>
-      <c r="O68" s="15">
-        <v>2033</v>
-      </c>
-      <c r="P68" s="15">
-        <v>2034</v>
-      </c>
-      <c r="Q68" s="15">
-        <v>2035</v>
-      </c>
-      <c r="R68" s="15">
-        <v>2036</v>
-      </c>
-      <c r="S68" s="15">
-        <v>2037</v>
-      </c>
-      <c r="T68" s="15">
-        <v>2038</v>
-      </c>
-      <c r="U68" s="15">
-        <v>2039</v>
-      </c>
-      <c r="V68" s="15">
-        <v>2040</v>
-      </c>
-      <c r="W68" s="15">
-        <v>2041</v>
-      </c>
-      <c r="X68" s="15">
-        <v>2042</v>
-      </c>
-      <c r="Y68" s="15">
-        <v>2043</v>
-      </c>
-      <c r="Z68" s="15">
-        <v>2044</v>
-      </c>
-      <c r="AA68" s="15">
-        <v>2045</v>
-      </c>
-      <c r="AB68" s="15">
-        <v>2046</v>
-      </c>
-      <c r="AC68" s="15">
-        <v>2047</v>
-      </c>
-      <c r="AD68" s="15">
-        <v>2048</v>
-      </c>
-      <c r="AE68" s="15">
-        <v>2049</v>
-      </c>
-      <c r="AF68" s="15">
-        <v>2050</v>
+        <v>956</v>
       </c>
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A69" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="15">
-        <v>4.0288390000000002E-3</v>
-      </c>
-      <c r="C69" s="15">
-        <v>7.4906770000000003E-3</v>
-      </c>
-      <c r="D69" s="15">
-        <v>1.3517357000000001E-2</v>
-      </c>
-      <c r="E69" s="15">
-        <v>2.2982546E-2</v>
-      </c>
-      <c r="F69" s="15">
-        <v>3.6100624999999997E-2</v>
-      </c>
-      <c r="G69" s="15">
-        <v>5.1007505000000002E-2</v>
-      </c>
-      <c r="H69" s="15">
-        <v>6.5037979999999995E-2</v>
-      </c>
-      <c r="I69" s="15">
-        <v>7.4050884999999997E-2</v>
-      </c>
-      <c r="J69" s="15">
-        <v>7.5902622000000003E-2</v>
-      </c>
-      <c r="K69" s="15">
-        <v>7.9969093000000005E-2</v>
-      </c>
-      <c r="L69" s="15">
-        <v>8.5852278000000004E-2</v>
-      </c>
-      <c r="M69" s="15">
-        <v>0.115342836</v>
-      </c>
-      <c r="N69" s="15">
-        <v>0.12811123299999999</v>
-      </c>
-      <c r="O69" s="15">
-        <v>0.14218904299999999</v>
-      </c>
-      <c r="P69" s="15">
-        <v>0.15715570200000001</v>
-      </c>
-      <c r="Q69" s="15">
-        <v>0.17312130100000001</v>
-      </c>
-      <c r="R69" s="15">
-        <v>0.18486860099999999</v>
-      </c>
-      <c r="S69" s="15">
-        <v>0.194230549</v>
-      </c>
-      <c r="T69" s="15">
-        <v>0.200844037</v>
-      </c>
-      <c r="U69" s="15">
-        <v>0.20479752200000001</v>
-      </c>
-      <c r="V69" s="15">
-        <v>0.20639531</v>
-      </c>
-      <c r="W69" s="15">
-        <v>0.207285109</v>
-      </c>
-      <c r="X69" s="15">
-        <v>0.205884558</v>
-      </c>
-      <c r="Y69" s="15">
-        <v>0.203850332</v>
-      </c>
-      <c r="Z69" s="15">
-        <v>0.20227350999999999</v>
-      </c>
-      <c r="AA69" s="15">
-        <v>0.201661221</v>
-      </c>
-      <c r="AB69" s="15">
-        <v>0.202610965</v>
-      </c>
-      <c r="AC69" s="15">
-        <v>0.20489760400000001</v>
-      </c>
-      <c r="AD69" s="15">
-        <v>0.20845095499999999</v>
-      </c>
-      <c r="AE69" s="15">
-        <v>0.21348747400000001</v>
-      </c>
-      <c r="AF69" s="15">
-        <v>0.22004099999999999</v>
+        <v>957</v>
       </c>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A71" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" s="15">
-        <v>3</v>
-      </c>
-      <c r="C71" s="15">
-        <v>3</v>
-      </c>
-      <c r="D71" s="15">
-        <v>3</v>
-      </c>
-      <c r="E71" s="15">
-        <v>3</v>
-      </c>
-      <c r="F71" s="15">
-        <v>3</v>
-      </c>
-      <c r="G71" s="15">
-        <v>3</v>
-      </c>
-      <c r="H71" s="15">
-        <v>3</v>
-      </c>
-      <c r="I71" s="15">
-        <v>3</v>
-      </c>
-      <c r="J71" s="15">
-        <v>3</v>
-      </c>
-      <c r="K71" s="15">
-        <v>3</v>
-      </c>
-      <c r="L71" s="15">
-        <v>3</v>
-      </c>
-      <c r="M71" s="15">
-        <v>3</v>
-      </c>
-      <c r="N71" s="15">
-        <v>3</v>
-      </c>
-      <c r="O71" s="15">
-        <v>3</v>
-      </c>
-      <c r="P71" s="15">
-        <v>3</v>
-      </c>
-      <c r="Q71" s="15">
-        <v>3</v>
-      </c>
-      <c r="R71" s="15">
-        <v>3</v>
-      </c>
-      <c r="S71" s="15">
-        <v>3</v>
-      </c>
-      <c r="T71" s="15">
-        <v>3</v>
-      </c>
-      <c r="U71" s="15">
-        <v>3</v>
-      </c>
-      <c r="V71" s="15">
-        <v>3</v>
-      </c>
-      <c r="W71" s="15">
-        <v>3</v>
-      </c>
-      <c r="X71" s="15">
-        <v>3</v>
-      </c>
-      <c r="Y71" s="15">
-        <v>3</v>
-      </c>
-      <c r="Z71" s="15">
-        <v>3</v>
-      </c>
-      <c r="AA71" s="15">
-        <v>3</v>
-      </c>
-      <c r="AB71" s="15">
-        <v>3</v>
-      </c>
-      <c r="AC71" s="15">
-        <v>3</v>
-      </c>
-      <c r="AD71" s="15">
-        <v>3</v>
-      </c>
-      <c r="AE71" s="15">
-        <v>3</v>
-      </c>
-      <c r="AF71" s="15">
-        <v>3</v>
+        <v>958</v>
+      </c>
+      <c r="F70" s="15">
+        <f t="shared" ref="F70:J70" si="4">G70-0.005</f>
+        <v>4.9999999999999984E-3</v>
+      </c>
+      <c r="G70" s="15">
+        <f t="shared" si="4"/>
+        <v>9.9999999999999985E-3</v>
+      </c>
+      <c r="H70" s="15">
+        <f t="shared" si="4"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I70" s="15">
+        <f t="shared" si="4"/>
+        <v>0.02</v>
+      </c>
+      <c r="J70" s="15">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K70" s="15">
+        <f>L70-0.005</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="L70" s="15">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A72" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="15">
-        <v>3</v>
-      </c>
-      <c r="C72" s="15">
-        <v>3</v>
-      </c>
-      <c r="D72" s="15">
-        <v>3</v>
-      </c>
-      <c r="E72" s="15">
-        <v>3</v>
-      </c>
-      <c r="F72" s="15">
-        <v>3</v>
-      </c>
-      <c r="G72" s="15">
-        <v>3</v>
-      </c>
-      <c r="H72" s="15">
-        <v>3</v>
-      </c>
-      <c r="I72" s="15">
-        <v>3</v>
-      </c>
-      <c r="J72" s="15">
-        <v>3</v>
-      </c>
-      <c r="K72" s="15">
-        <v>3</v>
-      </c>
-      <c r="L72" s="15">
-        <v>3</v>
-      </c>
-      <c r="M72" s="15">
-        <v>3</v>
-      </c>
-      <c r="N72" s="15">
-        <v>3</v>
-      </c>
-      <c r="O72" s="15">
-        <v>3</v>
-      </c>
-      <c r="P72" s="15">
-        <v>3</v>
-      </c>
-      <c r="Q72" s="15">
-        <v>3</v>
-      </c>
-      <c r="R72" s="15">
-        <v>3</v>
-      </c>
-      <c r="S72" s="15">
-        <v>3</v>
-      </c>
-      <c r="T72" s="15">
-        <v>3</v>
-      </c>
-      <c r="U72" s="15">
-        <v>3</v>
-      </c>
-      <c r="V72" s="15">
-        <v>3</v>
-      </c>
-      <c r="W72" s="15">
-        <v>3</v>
-      </c>
-      <c r="X72" s="15">
-        <v>3</v>
-      </c>
-      <c r="Y72" s="15">
-        <v>3</v>
-      </c>
-      <c r="Z72" s="15">
-        <v>3</v>
-      </c>
-      <c r="AA72" s="15">
-        <v>3</v>
-      </c>
-      <c r="AB72" s="15">
-        <v>3</v>
-      </c>
-      <c r="AC72" s="15">
-        <v>3</v>
-      </c>
-      <c r="AD72" s="15">
-        <v>3</v>
-      </c>
-      <c r="AE72" s="15">
-        <v>3</v>
-      </c>
-      <c r="AF72" s="15">
-        <v>3</v>
+      <c r="A72" s="14" t="s">
+        <v>952</v>
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="B73" s="15">
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="C73" s="15">
-        <v>0</v>
+        <v>2021</v>
       </c>
       <c r="D73" s="15">
-        <v>0</v>
+        <v>2022</v>
       </c>
       <c r="E73" s="15">
-        <v>0</v>
+        <v>2023</v>
       </c>
       <c r="F73" s="15">
-        <v>0</v>
+        <v>2024</v>
       </c>
       <c r="G73" s="15">
-        <v>0</v>
+        <v>2025</v>
       </c>
       <c r="H73" s="15">
-        <v>0</v>
+        <v>2026</v>
       </c>
       <c r="I73" s="15">
-        <v>0</v>
+        <v>2027</v>
       </c>
       <c r="J73" s="15">
-        <v>0</v>
+        <v>2028</v>
       </c>
       <c r="K73" s="15">
-        <v>0</v>
+        <v>2029</v>
       </c>
       <c r="L73" s="15">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="M73" s="15">
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="N73" s="15">
-        <v>0</v>
+        <v>2032</v>
       </c>
       <c r="O73" s="15">
-        <v>0</v>
+        <v>2033</v>
       </c>
       <c r="P73" s="15">
-        <v>0</v>
+        <v>2034</v>
       </c>
       <c r="Q73" s="15">
-        <v>0</v>
+        <v>2035</v>
       </c>
       <c r="R73" s="15">
-        <v>0</v>
+        <v>2036</v>
       </c>
       <c r="S73" s="15">
-        <v>0</v>
+        <v>2037</v>
       </c>
       <c r="T73" s="15">
-        <v>0</v>
+        <v>2038</v>
       </c>
       <c r="U73" s="15">
-        <v>0</v>
+        <v>2039</v>
       </c>
       <c r="V73" s="15">
-        <v>0</v>
+        <v>2040</v>
       </c>
       <c r="W73" s="15">
-        <v>0</v>
+        <v>2041</v>
       </c>
       <c r="X73" s="15">
-        <v>0</v>
+        <v>2042</v>
       </c>
       <c r="Y73" s="15">
-        <v>0</v>
+        <v>2043</v>
       </c>
       <c r="Z73" s="15">
-        <v>0</v>
+        <v>2044</v>
       </c>
       <c r="AA73" s="15">
-        <v>0</v>
+        <v>2045</v>
       </c>
       <c r="AB73" s="15">
-        <v>0</v>
+        <v>2046</v>
       </c>
       <c r="AC73" s="15">
-        <v>0</v>
+        <v>2047</v>
       </c>
       <c r="AD73" s="15">
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="AE73" s="15">
-        <v>0</v>
+        <v>2049</v>
       </c>
       <c r="AF73" s="15">
-        <v>0</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A74" s="15" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="B74" s="15">
-        <v>0</v>
+        <v>4.0288390000000002E-3</v>
       </c>
       <c r="C74" s="15">
-        <v>0</v>
+        <v>7.4906770000000003E-3</v>
       </c>
       <c r="D74" s="15">
-        <v>0</v>
+        <v>1.3517357000000001E-2</v>
       </c>
       <c r="E74" s="15">
-        <v>0</v>
+        <v>2.2982546E-2</v>
       </c>
       <c r="F74" s="15">
-        <v>0</v>
+        <v>3.6100624999999997E-2</v>
       </c>
       <c r="G74" s="15">
-        <v>0</v>
+        <v>5.1007505000000002E-2</v>
       </c>
       <c r="H74" s="15">
-        <v>0</v>
+        <v>6.5037979999999995E-2</v>
       </c>
       <c r="I74" s="15">
-        <v>0</v>
+        <v>7.4050884999999997E-2</v>
       </c>
       <c r="J74" s="15">
-        <v>0</v>
+        <v>7.5902622000000003E-2</v>
       </c>
       <c r="K74" s="15">
-        <v>0</v>
+        <v>7.9969093000000005E-2</v>
       </c>
       <c r="L74" s="15">
-        <v>0</v>
+        <v>8.5852278000000004E-2</v>
       </c>
       <c r="M74" s="15">
-        <v>0</v>
+        <v>0.115342836</v>
       </c>
       <c r="N74" s="15">
-        <v>0</v>
+        <v>0.12811123299999999</v>
       </c>
       <c r="O74" s="15">
-        <v>0</v>
+        <v>0.14218904299999999</v>
       </c>
       <c r="P74" s="15">
-        <v>0</v>
+        <v>0.15715570200000001</v>
       </c>
       <c r="Q74" s="15">
-        <v>0</v>
+        <v>0.17312130100000001</v>
       </c>
       <c r="R74" s="15">
-        <v>0</v>
+        <v>0.18486860099999999</v>
       </c>
       <c r="S74" s="15">
-        <v>0</v>
+        <v>0.194230549</v>
       </c>
       <c r="T74" s="15">
-        <v>0</v>
+        <v>0.200844037</v>
       </c>
       <c r="U74" s="15">
-        <v>0</v>
+        <v>0.20479752200000001</v>
       </c>
       <c r="V74" s="15">
-        <v>0</v>
+        <v>0.20639531</v>
       </c>
       <c r="W74" s="15">
-        <v>0</v>
+        <v>0.207285109</v>
       </c>
       <c r="X74" s="15">
-        <v>0</v>
+        <v>0.205884558</v>
       </c>
       <c r="Y74" s="15">
-        <v>0</v>
+        <v>0.203850332</v>
       </c>
       <c r="Z74" s="15">
-        <v>0</v>
+        <v>0.20227350999999999</v>
       </c>
       <c r="AA74" s="15">
-        <v>0</v>
+        <v>0.201661221</v>
       </c>
       <c r="AB74" s="15">
-        <v>0</v>
+        <v>0.202610965</v>
       </c>
       <c r="AC74" s="15">
-        <v>0</v>
+        <v>0.20489760400000001</v>
       </c>
       <c r="AD74" s="15">
-        <v>0</v>
+        <v>0.20845095499999999</v>
       </c>
       <c r="AE74" s="15">
-        <v>0</v>
+        <v>0.21348747400000001</v>
       </c>
       <c r="AF74" s="15">
-        <v>0</v>
+        <v>0.22004099999999999</v>
       </c>
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A75" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="15">
-        <v>0</v>
-      </c>
-      <c r="C75" s="15">
-        <v>0</v>
-      </c>
-      <c r="D75" s="15">
-        <v>0</v>
-      </c>
-      <c r="E75" s="15">
-        <v>0</v>
-      </c>
-      <c r="F75" s="15">
-        <v>0</v>
-      </c>
-      <c r="G75" s="15">
-        <v>0</v>
-      </c>
-      <c r="H75" s="15">
-        <v>0</v>
-      </c>
-      <c r="I75" s="15">
-        <v>0</v>
-      </c>
-      <c r="J75" s="15">
-        <v>0</v>
-      </c>
-      <c r="K75" s="15">
-        <v>0</v>
-      </c>
-      <c r="L75" s="15">
-        <v>0</v>
-      </c>
-      <c r="M75" s="15">
-        <v>0</v>
-      </c>
-      <c r="N75" s="15">
-        <v>0</v>
-      </c>
-      <c r="O75" s="15">
-        <v>0</v>
-      </c>
-      <c r="P75" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q75" s="15">
-        <v>0</v>
-      </c>
-      <c r="R75" s="15">
-        <v>0</v>
-      </c>
-      <c r="S75" s="15">
-        <v>0</v>
-      </c>
-      <c r="T75" s="15">
-        <v>0</v>
-      </c>
-      <c r="U75" s="15">
-        <v>0</v>
-      </c>
-      <c r="V75" s="15">
-        <v>0</v>
-      </c>
-      <c r="W75" s="15">
-        <v>0</v>
-      </c>
-      <c r="X75" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y75" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z75" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA75" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB75" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC75" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD75" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE75" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF75" s="15">
-        <v>0</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A76" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="15">
+        <v>3</v>
+      </c>
+      <c r="C76" s="15">
+        <v>3</v>
+      </c>
+      <c r="D76" s="15">
+        <v>3</v>
+      </c>
+      <c r="E76" s="15">
+        <v>3</v>
+      </c>
+      <c r="F76" s="15">
+        <v>3</v>
+      </c>
+      <c r="G76" s="15">
+        <v>3</v>
+      </c>
+      <c r="H76" s="15">
+        <v>3</v>
+      </c>
+      <c r="I76" s="15">
+        <v>3</v>
+      </c>
+      <c r="J76" s="15">
+        <v>3</v>
+      </c>
+      <c r="K76" s="15">
+        <v>3</v>
+      </c>
+      <c r="L76" s="15">
+        <v>3</v>
+      </c>
+      <c r="M76" s="15">
+        <v>3</v>
+      </c>
+      <c r="N76" s="15">
+        <v>3</v>
+      </c>
+      <c r="O76" s="15">
+        <v>3</v>
+      </c>
+      <c r="P76" s="15">
+        <v>3</v>
+      </c>
+      <c r="Q76" s="15">
+        <v>3</v>
+      </c>
+      <c r="R76" s="15">
+        <v>3</v>
+      </c>
+      <c r="S76" s="15">
+        <v>3</v>
+      </c>
+      <c r="T76" s="15">
+        <v>3</v>
+      </c>
+      <c r="U76" s="15">
+        <v>3</v>
+      </c>
+      <c r="V76" s="15">
+        <v>3</v>
+      </c>
+      <c r="W76" s="15">
+        <v>3</v>
+      </c>
+      <c r="X76" s="15">
+        <v>3</v>
+      </c>
+      <c r="Y76" s="15">
+        <v>3</v>
+      </c>
+      <c r="Z76" s="15">
+        <v>3</v>
+      </c>
+      <c r="AA76" s="15">
+        <v>3</v>
+      </c>
+      <c r="AB76" s="15">
+        <v>3</v>
+      </c>
+      <c r="AC76" s="15">
+        <v>3</v>
+      </c>
+      <c r="AD76" s="15">
+        <v>3</v>
+      </c>
+      <c r="AE76" s="15">
+        <v>3</v>
+      </c>
+      <c r="AF76" s="15">
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A77" s="15" t="s">
-        <v>953</v>
+        <v>4</v>
+      </c>
+      <c r="B77" s="15">
+        <v>3</v>
+      </c>
+      <c r="C77" s="15">
+        <v>3</v>
+      </c>
+      <c r="D77" s="15">
+        <v>3</v>
+      </c>
+      <c r="E77" s="15">
+        <v>3</v>
+      </c>
+      <c r="F77" s="15">
+        <v>3</v>
+      </c>
+      <c r="G77" s="15">
+        <v>3</v>
+      </c>
+      <c r="H77" s="15">
+        <v>3</v>
+      </c>
+      <c r="I77" s="15">
+        <v>3</v>
+      </c>
+      <c r="J77" s="15">
+        <v>3</v>
+      </c>
+      <c r="K77" s="15">
+        <v>3</v>
+      </c>
+      <c r="L77" s="15">
+        <v>3</v>
+      </c>
+      <c r="M77" s="15">
+        <v>3</v>
+      </c>
+      <c r="N77" s="15">
+        <v>3</v>
+      </c>
+      <c r="O77" s="15">
+        <v>3</v>
+      </c>
+      <c r="P77" s="15">
+        <v>3</v>
+      </c>
+      <c r="Q77" s="15">
+        <v>3</v>
+      </c>
+      <c r="R77" s="15">
+        <v>3</v>
+      </c>
+      <c r="S77" s="15">
+        <v>3</v>
+      </c>
+      <c r="T77" s="15">
+        <v>3</v>
+      </c>
+      <c r="U77" s="15">
+        <v>3</v>
+      </c>
+      <c r="V77" s="15">
+        <v>3</v>
+      </c>
+      <c r="W77" s="15">
+        <v>3</v>
+      </c>
+      <c r="X77" s="15">
+        <v>3</v>
+      </c>
+      <c r="Y77" s="15">
+        <v>3</v>
+      </c>
+      <c r="Z77" s="15">
+        <v>3</v>
+      </c>
+      <c r="AA77" s="15">
+        <v>3</v>
+      </c>
+      <c r="AB77" s="15">
+        <v>3</v>
+      </c>
+      <c r="AC77" s="15">
+        <v>3</v>
+      </c>
+      <c r="AD77" s="15">
+        <v>3</v>
+      </c>
+      <c r="AE77" s="15">
+        <v>3</v>
+      </c>
+      <c r="AF77" s="15">
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="B78" s="15">
-        <v>2020</v>
+        <v>0</v>
       </c>
       <c r="C78" s="15">
-        <v>2021</v>
+        <v>0</v>
       </c>
       <c r="D78" s="15">
-        <v>2022</v>
+        <v>0</v>
       </c>
       <c r="E78" s="15">
-        <v>2023</v>
+        <v>0</v>
       </c>
       <c r="F78" s="15">
-        <v>2024</v>
+        <v>0</v>
       </c>
       <c r="G78" s="15">
-        <v>2025</v>
+        <v>0</v>
       </c>
       <c r="H78" s="15">
-        <v>2026</v>
+        <v>0</v>
       </c>
       <c r="I78" s="15">
-        <v>2027</v>
+        <v>0</v>
       </c>
       <c r="J78" s="15">
-        <v>2028</v>
+        <v>0</v>
       </c>
       <c r="K78" s="15">
-        <v>2029</v>
+        <v>0</v>
       </c>
       <c r="L78" s="15">
-        <v>2030</v>
+        <v>0</v>
       </c>
       <c r="M78" s="15">
-        <v>2031</v>
+        <v>0</v>
       </c>
       <c r="N78" s="15">
-        <v>2032</v>
+        <v>0</v>
       </c>
       <c r="O78" s="15">
-        <v>2033</v>
+        <v>0</v>
       </c>
       <c r="P78" s="15">
-        <v>2034</v>
+        <v>0</v>
       </c>
       <c r="Q78" s="15">
-        <v>2035</v>
+        <v>0</v>
       </c>
       <c r="R78" s="15">
-        <v>2036</v>
+        <v>0</v>
       </c>
       <c r="S78" s="15">
-        <v>2037</v>
+        <v>0</v>
       </c>
       <c r="T78" s="15">
-        <v>2038</v>
+        <v>0</v>
       </c>
       <c r="U78" s="15">
-        <v>2039</v>
+        <v>0</v>
       </c>
       <c r="V78" s="15">
-        <v>2040</v>
+        <v>0</v>
       </c>
       <c r="W78" s="15">
-        <v>2041</v>
+        <v>0</v>
       </c>
       <c r="X78" s="15">
-        <v>2042</v>
+        <v>0</v>
       </c>
       <c r="Y78" s="15">
-        <v>2043</v>
+        <v>0</v>
       </c>
       <c r="Z78" s="15">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="AA78" s="15">
-        <v>2045</v>
+        <v>0</v>
       </c>
       <c r="AB78" s="15">
-        <v>2046</v>
+        <v>0</v>
       </c>
       <c r="AC78" s="15">
-        <v>2047</v>
+        <v>0</v>
       </c>
       <c r="AD78" s="15">
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="AE78" s="15">
-        <v>2049</v>
+        <v>0</v>
       </c>
       <c r="AF78" s="15">
-        <v>2050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="B79" s="15">
-        <v>2.162813E-3</v>
+        <v>0</v>
       </c>
       <c r="C79" s="15">
-        <v>2.3154429999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="D79" s="15">
-        <v>3.8036620000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="E79" s="15">
-        <v>5.3024580000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="F79" s="15">
-        <v>6.8161840000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="G79" s="15">
-        <v>8.3520650000000005E-3</v>
+        <v>0</v>
       </c>
       <c r="H79" s="15">
-        <v>9.9196909999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="I79" s="15">
-        <v>1.1533804E-2</v>
+        <v>0</v>
       </c>
       <c r="J79" s="15">
-        <v>1.3212750000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="K79" s="15">
-        <v>1.4978709E-2</v>
+        <v>0</v>
       </c>
       <c r="L79" s="15">
-        <v>1.6867157000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="M79" s="15">
-        <v>1.7452430000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="N79" s="15">
-        <v>1.8252092000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="O79" s="15">
-        <v>1.9309627999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="P79" s="15">
-        <v>2.0645547E-2</v>
+        <v>0</v>
       </c>
       <c r="Q79" s="15">
-        <v>2.227985E-2</v>
+        <v>0</v>
       </c>
       <c r="R79" s="15">
-        <v>2.4351382000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="S79" s="15">
-        <v>2.6780347999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="T79" s="15">
-        <v>2.9592798E-2</v>
+        <v>0</v>
       </c>
       <c r="U79" s="15">
-        <v>3.2960165999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="V79" s="15">
-        <v>3.7044072999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="W79" s="15">
-        <v>4.2587001999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="X79" s="15">
-        <v>4.8824688999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Y79" s="15">
-        <v>5.5696411000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="Z79" s="15">
-        <v>6.2507718000000004E-2</v>
+        <v>0</v>
       </c>
       <c r="AA79" s="15">
-        <v>6.8291605000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="AB79" s="15">
-        <v>7.2692810999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="AC79" s="15">
-        <v>7.5988175000000005E-2</v>
+        <v>0</v>
       </c>
       <c r="AD79" s="15">
-        <v>7.8326194000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="AE79" s="15">
-        <v>8.0239419000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="AF79" s="15">
-        <v>8.1928860000000006E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A80" s="15" t="s">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="B80" s="15">
-        <v>7.3589795E-2</v>
+        <v>0</v>
       </c>
       <c r="C80" s="15">
-        <v>7.3995889999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="D80" s="15">
-        <v>7.3941642000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="E80" s="15">
-        <v>7.3765467000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="F80" s="15">
-        <v>7.3390425999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="G80" s="15">
-        <v>7.2711755000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="H80" s="15">
-        <v>7.1783712999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="I80" s="15">
-        <v>7.0928409999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="J80" s="15">
-        <v>7.0469529000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="K80" s="15">
-        <v>7.0480107E-2</v>
+        <v>0</v>
       </c>
       <c r="L80" s="15">
-        <v>7.0984199999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="M80" s="15">
-        <v>7.1919686999999996E-2</v>
+        <v>0</v>
       </c>
       <c r="N80" s="15">
-        <v>7.3416383000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="O80" s="15">
-        <v>7.5395217E-2</v>
+        <v>0</v>
       </c>
       <c r="P80" s="15">
-        <v>7.7468259999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="Q80" s="15">
-        <v>7.9363059E-2</v>
+        <v>0</v>
       </c>
       <c r="R80" s="15">
-        <v>8.2309397000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="S80" s="15">
-        <v>8.5071710999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="T80" s="15">
-        <v>8.7719454000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="U80" s="15">
-        <v>9.1121837999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="V80" s="15">
-        <v>9.5418878999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="W80" s="15">
-        <v>0.103777671</v>
+        <v>0</v>
       </c>
       <c r="X80" s="15">
-        <v>0.111585432</v>
+        <v>0</v>
       </c>
       <c r="Y80" s="15">
-        <v>0.12034946000000001</v>
+        <v>0</v>
       </c>
       <c r="Z80" s="15">
-        <v>0.12938412199999999</v>
+        <v>0</v>
       </c>
       <c r="AA80" s="15">
-        <v>0.13682857200000001</v>
+        <v>0</v>
       </c>
       <c r="AB80" s="15">
-        <v>0.14210099500000001</v>
+        <v>0</v>
       </c>
       <c r="AC80" s="15">
-        <v>0.145822912</v>
+        <v>0</v>
       </c>
       <c r="AD80" s="15">
-        <v>0.14804408299999999</v>
+        <v>0</v>
       </c>
       <c r="AE80" s="15">
-        <v>0.14978561500000001</v>
+        <v>0</v>
       </c>
       <c r="AF80" s="15">
-        <v>0.15130775599999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A81" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="15">
-        <v>0</v>
-      </c>
-      <c r="C81" s="15">
-        <v>0</v>
-      </c>
-      <c r="D81" s="15">
-        <v>0</v>
-      </c>
-      <c r="E81" s="15">
-        <v>0</v>
-      </c>
-      <c r="F81" s="15">
-        <v>0</v>
-      </c>
-      <c r="G81" s="15">
-        <v>0</v>
-      </c>
-      <c r="H81" s="15">
-        <v>0</v>
-      </c>
-      <c r="I81" s="15">
-        <v>0</v>
-      </c>
-      <c r="J81" s="15">
-        <v>0</v>
-      </c>
-      <c r="K81" s="15">
-        <v>0</v>
-      </c>
-      <c r="L81" s="15">
-        <v>0</v>
-      </c>
-      <c r="M81" s="15">
-        <v>0</v>
-      </c>
-      <c r="N81" s="15">
-        <v>0</v>
-      </c>
-      <c r="O81" s="15">
-        <v>0</v>
-      </c>
-      <c r="P81" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q81" s="15">
-        <v>0</v>
-      </c>
-      <c r="R81" s="15">
-        <v>0</v>
-      </c>
-      <c r="S81" s="15">
-        <v>0</v>
-      </c>
-      <c r="T81" s="15">
-        <v>0</v>
-      </c>
-      <c r="U81" s="15">
-        <v>0</v>
-      </c>
-      <c r="V81" s="15">
-        <v>0</v>
-      </c>
-      <c r="W81" s="15">
-        <v>0</v>
-      </c>
-      <c r="X81" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y81" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z81" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA81" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB81" s="15">
-        <v>0</v>
-      </c>
-      <c r="AC81" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD81" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE81" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF81" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A82" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="15">
-        <v>5</v>
-      </c>
-      <c r="C82" s="15">
-        <v>5</v>
-      </c>
-      <c r="D82" s="15">
-        <v>5</v>
-      </c>
-      <c r="E82" s="15">
-        <v>5</v>
-      </c>
-      <c r="F82" s="15">
-        <v>5</v>
-      </c>
-      <c r="G82" s="15">
-        <v>5</v>
-      </c>
-      <c r="H82" s="15">
-        <v>5</v>
-      </c>
-      <c r="I82" s="15">
-        <v>5</v>
-      </c>
-      <c r="J82" s="15">
-        <v>5</v>
-      </c>
-      <c r="K82" s="15">
-        <v>5</v>
-      </c>
-      <c r="L82" s="15">
-        <v>5</v>
-      </c>
-      <c r="M82" s="15">
-        <v>5</v>
-      </c>
-      <c r="N82" s="15">
-        <v>5</v>
-      </c>
-      <c r="O82" s="15">
-        <v>5</v>
-      </c>
-      <c r="P82" s="15">
-        <v>5</v>
-      </c>
-      <c r="Q82" s="15">
-        <v>5</v>
-      </c>
-      <c r="R82" s="15">
-        <v>5</v>
-      </c>
-      <c r="S82" s="15">
-        <v>5</v>
-      </c>
-      <c r="T82" s="15">
-        <v>5</v>
-      </c>
-      <c r="U82" s="15">
-        <v>5</v>
-      </c>
-      <c r="V82" s="15">
-        <v>5</v>
-      </c>
-      <c r="W82" s="15">
-        <v>5</v>
-      </c>
-      <c r="X82" s="15">
-        <v>5</v>
-      </c>
-      <c r="Y82" s="15">
-        <v>5</v>
-      </c>
-      <c r="Z82" s="15">
-        <v>5</v>
-      </c>
-      <c r="AA82" s="15">
-        <v>5</v>
-      </c>
-      <c r="AB82" s="15">
-        <v>5</v>
-      </c>
-      <c r="AC82" s="15">
-        <v>5</v>
-      </c>
-      <c r="AD82" s="15">
-        <v>5</v>
-      </c>
-      <c r="AE82" s="15">
-        <v>5</v>
-      </c>
-      <c r="AF82" s="15">
-        <v>5</v>
+        <v>953</v>
       </c>
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A83" s="15" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="B83" s="15">
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="C83" s="15">
-        <v>0</v>
+        <v>2021</v>
       </c>
       <c r="D83" s="15">
-        <v>0</v>
+        <v>2022</v>
       </c>
       <c r="E83" s="15">
-        <v>0</v>
+        <v>2023</v>
       </c>
       <c r="F83" s="15">
-        <v>0</v>
+        <v>2024</v>
       </c>
       <c r="G83" s="15">
-        <v>0</v>
+        <v>2025</v>
       </c>
       <c r="H83" s="15">
-        <v>0</v>
+        <v>2026</v>
       </c>
       <c r="I83" s="15">
-        <v>0</v>
+        <v>2027</v>
       </c>
       <c r="J83" s="15">
-        <v>0</v>
+        <v>2028</v>
       </c>
       <c r="K83" s="15">
-        <v>0</v>
+        <v>2029</v>
       </c>
       <c r="L83" s="15">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="M83" s="15">
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="N83" s="15">
-        <v>0</v>
+        <v>2032</v>
       </c>
       <c r="O83" s="15">
-        <v>0</v>
+        <v>2033</v>
       </c>
       <c r="P83" s="15">
-        <v>0</v>
+        <v>2034</v>
       </c>
       <c r="Q83" s="15">
-        <v>0</v>
+        <v>2035</v>
       </c>
       <c r="R83" s="15">
-        <v>0</v>
+        <v>2036</v>
       </c>
       <c r="S83" s="15">
-        <v>0</v>
+        <v>2037</v>
       </c>
       <c r="T83" s="15">
-        <v>0</v>
+        <v>2038</v>
       </c>
       <c r="U83" s="15">
-        <v>0</v>
+        <v>2039</v>
       </c>
       <c r="V83" s="15">
-        <v>0</v>
+        <v>2040</v>
       </c>
       <c r="W83" s="15">
-        <v>0</v>
+        <v>2041</v>
       </c>
       <c r="X83" s="15">
-        <v>0</v>
+        <v>2042</v>
       </c>
       <c r="Y83" s="15">
-        <v>0</v>
+        <v>2043</v>
       </c>
       <c r="Z83" s="15">
-        <v>0</v>
+        <v>2044</v>
       </c>
       <c r="AA83" s="15">
-        <v>0</v>
+        <v>2045</v>
       </c>
       <c r="AB83" s="15">
-        <v>0</v>
+        <v>2046</v>
       </c>
       <c r="AC83" s="15">
-        <v>0</v>
+        <v>2047</v>
       </c>
       <c r="AD83" s="15">
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="AE83" s="15">
-        <v>0</v>
+        <v>2049</v>
       </c>
       <c r="AF83" s="15">
-        <v>0</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="84" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="B84" s="15">
-        <v>0</v>
+        <v>2.162813E-3</v>
       </c>
       <c r="C84" s="15">
-        <v>0</v>
+        <v>2.3154429999999999E-3</v>
       </c>
       <c r="D84" s="15">
-        <v>0</v>
+        <v>3.8036620000000002E-3</v>
       </c>
       <c r="E84" s="15">
-        <v>0</v>
+        <v>5.3024580000000003E-3</v>
       </c>
       <c r="F84" s="15">
-        <v>0</v>
+        <v>6.8161840000000003E-3</v>
       </c>
       <c r="G84" s="15">
-        <v>0</v>
+        <v>8.3520650000000005E-3</v>
       </c>
       <c r="H84" s="15">
-        <v>0</v>
+        <v>9.9196909999999996E-3</v>
       </c>
       <c r="I84" s="15">
-        <v>0</v>
+        <v>1.1533804E-2</v>
       </c>
       <c r="J84" s="15">
-        <v>0</v>
+        <v>1.3212750000000001E-2</v>
       </c>
       <c r="K84" s="15">
-        <v>0</v>
+        <v>1.4978709E-2</v>
       </c>
       <c r="L84" s="15">
-        <v>0</v>
+        <v>1.6867157000000001E-2</v>
       </c>
       <c r="M84" s="15">
-        <v>0</v>
+        <v>1.7452430000000001E-2</v>
       </c>
       <c r="N84" s="15">
-        <v>0</v>
+        <v>1.8252092000000001E-2</v>
       </c>
       <c r="O84" s="15">
-        <v>0</v>
+        <v>1.9309627999999999E-2</v>
       </c>
       <c r="P84" s="15">
-        <v>0</v>
+        <v>2.0645547E-2</v>
       </c>
       <c r="Q84" s="15">
-        <v>0</v>
+        <v>2.227985E-2</v>
       </c>
       <c r="R84" s="15">
-        <v>0</v>
+        <v>2.4351382000000001E-2</v>
       </c>
       <c r="S84" s="15">
-        <v>0</v>
+        <v>2.6780347999999999E-2</v>
       </c>
       <c r="T84" s="15">
-        <v>0</v>
+        <v>2.9592798E-2</v>
       </c>
       <c r="U84" s="15">
-        <v>0</v>
+        <v>3.2960165999999999E-2</v>
       </c>
       <c r="V84" s="15">
-        <v>0</v>
+        <v>3.7044072999999997E-2</v>
       </c>
       <c r="W84" s="15">
-        <v>0</v>
+        <v>4.2587001999999999E-2</v>
       </c>
       <c r="X84" s="15">
-        <v>0</v>
+        <v>4.8824688999999998E-2</v>
       </c>
       <c r="Y84" s="15">
-        <v>0</v>
+        <v>5.5696411000000001E-2</v>
       </c>
       <c r="Z84" s="15">
-        <v>0</v>
+        <v>6.2507718000000004E-2</v>
       </c>
       <c r="AA84" s="15">
-        <v>0</v>
+        <v>6.8291605000000005E-2</v>
       </c>
       <c r="AB84" s="15">
-        <v>0</v>
+        <v>7.2692810999999996E-2</v>
       </c>
       <c r="AC84" s="15">
-        <v>0</v>
+        <v>7.5988175000000005E-2</v>
       </c>
       <c r="AD84" s="15">
-        <v>0</v>
+        <v>7.8326194000000002E-2</v>
       </c>
       <c r="AE84" s="15">
-        <v>0</v>
+        <v>8.0239419000000006E-2</v>
       </c>
       <c r="AF84" s="15">
-        <v>0</v>
+        <v>8.1928860000000006E-2</v>
       </c>
     </row>
     <row r="85" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A85" s="15" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="B85" s="15">
-        <v>2.16E-3</v>
+        <v>7.3589795E-2</v>
       </c>
       <c r="C85" s="15">
-        <v>2.3154429999999999E-3</v>
+        <v>7.3995889999999995E-2</v>
       </c>
       <c r="D85" s="15">
-        <v>3.8036620000000002E-3</v>
+        <v>7.3941642000000002E-2</v>
       </c>
       <c r="E85" s="15">
-        <v>5.3024580000000003E-3</v>
+        <v>7.3765467000000001E-2</v>
       </c>
       <c r="F85" s="15">
-        <v>6.8161840000000003E-3</v>
+        <v>7.3390425999999995E-2</v>
       </c>
       <c r="G85" s="15">
-        <v>8.3520650000000005E-3</v>
+        <v>7.2711755000000003E-2</v>
       </c>
       <c r="H85" s="15">
-        <v>9.9196909999999996E-3</v>
+        <v>7.1783712999999999E-2</v>
       </c>
       <c r="I85" s="15">
-        <v>1.1533804E-2</v>
+        <v>7.0928409999999997E-2</v>
       </c>
       <c r="J85" s="15">
-        <v>1.3212750000000001E-2</v>
+        <v>7.0469529000000003E-2</v>
       </c>
       <c r="K85" s="15">
-        <v>1.4978709E-2</v>
+        <v>7.0480107E-2</v>
       </c>
       <c r="L85" s="15">
-        <v>1.6867157000000001E-2</v>
+        <v>7.0984199999999997E-2</v>
       </c>
       <c r="M85" s="15">
-        <v>1.7452430000000001E-2</v>
+        <v>7.1919686999999996E-2</v>
       </c>
       <c r="N85" s="15">
-        <v>1.8252092000000001E-2</v>
+        <v>7.3416383000000002E-2</v>
       </c>
       <c r="O85" s="15">
-        <v>1.9309627999999999E-2</v>
+        <v>7.5395217E-2</v>
       </c>
       <c r="P85" s="15">
-        <v>2.0645547E-2</v>
+        <v>7.7468259999999997E-2</v>
       </c>
       <c r="Q85" s="15">
-        <v>2.227985E-2</v>
+        <v>7.9363059E-2</v>
       </c>
       <c r="R85" s="15">
-        <v>2.4351382000000001E-2</v>
+        <v>8.2309397000000006E-2</v>
       </c>
       <c r="S85" s="15">
-        <v>2.6780347999999999E-2</v>
+        <v>8.5071710999999994E-2</v>
       </c>
       <c r="T85" s="15">
-        <v>2.9592798E-2</v>
+        <v>8.7719454000000002E-2</v>
       </c>
       <c r="U85" s="15">
-        <v>3.2960165999999999E-2</v>
+        <v>9.1121837999999997E-2</v>
       </c>
       <c r="V85" s="15">
-        <v>3.7044072999999997E-2</v>
+        <v>9.5418878999999998E-2</v>
       </c>
       <c r="W85" s="15">
-        <v>4.2587001999999999E-2</v>
+        <v>0.103777671</v>
       </c>
       <c r="X85" s="15">
-        <v>4.8824688999999998E-2</v>
+        <v>0.111585432</v>
       </c>
       <c r="Y85" s="15">
-        <v>5.5696411000000001E-2</v>
+        <v>0.12034946000000001</v>
       </c>
       <c r="Z85" s="15">
-        <v>6.2507718000000004E-2</v>
+        <v>0.12938412199999999</v>
       </c>
       <c r="AA85" s="15">
-        <v>6.8291605000000005E-2</v>
+        <v>0.13682857200000001</v>
       </c>
       <c r="AB85" s="15">
-        <v>7.2692810999999996E-2</v>
+        <v>0.14210099500000001</v>
       </c>
       <c r="AC85" s="15">
-        <v>7.5988175000000005E-2</v>
+        <v>0.145822912</v>
       </c>
       <c r="AD85" s="15">
-        <v>7.8326194000000002E-2</v>
+        <v>0.14804408299999999</v>
       </c>
       <c r="AE85" s="15">
-        <v>8.0239419000000006E-2</v>
+        <v>0.14978561500000001</v>
       </c>
       <c r="AF85" s="15">
-        <v>8.1928860000000006E-2</v>
+        <v>0.15130775599999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A86" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="15">
+        <v>0</v>
+      </c>
+      <c r="C86" s="15">
+        <v>0</v>
+      </c>
+      <c r="D86" s="15">
+        <v>0</v>
+      </c>
+      <c r="E86" s="15">
+        <v>0</v>
+      </c>
+      <c r="F86" s="15">
+        <v>0</v>
+      </c>
+      <c r="G86" s="15">
+        <v>0</v>
+      </c>
+      <c r="H86" s="15">
+        <v>0</v>
+      </c>
+      <c r="I86" s="15">
+        <v>0</v>
+      </c>
+      <c r="J86" s="15">
+        <v>0</v>
+      </c>
+      <c r="K86" s="15">
+        <v>0</v>
+      </c>
+      <c r="L86" s="15">
+        <v>0</v>
+      </c>
+      <c r="M86" s="15">
+        <v>0</v>
+      </c>
+      <c r="N86" s="15">
+        <v>0</v>
+      </c>
+      <c r="O86" s="15">
+        <v>0</v>
+      </c>
+      <c r="P86" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="15">
+        <v>0</v>
+      </c>
+      <c r="R86" s="15">
+        <v>0</v>
+      </c>
+      <c r="S86" s="15">
+        <v>0</v>
+      </c>
+      <c r="T86" s="15">
+        <v>0</v>
+      </c>
+      <c r="U86" s="15">
+        <v>0</v>
+      </c>
+      <c r="V86" s="15">
+        <v>0</v>
+      </c>
+      <c r="W86" s="15">
+        <v>0</v>
+      </c>
+      <c r="X86" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y86" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z86" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA86" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC86" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD86" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE86" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF86" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
-        <v>954</v>
+        <v>4</v>
+      </c>
+      <c r="B87" s="15">
+        <v>5</v>
+      </c>
+      <c r="C87" s="15">
+        <v>5</v>
+      </c>
+      <c r="D87" s="15">
+        <v>5</v>
+      </c>
+      <c r="E87" s="15">
+        <v>5</v>
+      </c>
+      <c r="F87" s="15">
+        <v>5</v>
+      </c>
+      <c r="G87" s="15">
+        <v>5</v>
+      </c>
+      <c r="H87" s="15">
+        <v>5</v>
+      </c>
+      <c r="I87" s="15">
+        <v>5</v>
+      </c>
+      <c r="J87" s="15">
+        <v>5</v>
+      </c>
+      <c r="K87" s="15">
+        <v>5</v>
+      </c>
+      <c r="L87" s="15">
+        <v>5</v>
+      </c>
+      <c r="M87" s="15">
+        <v>5</v>
+      </c>
+      <c r="N87" s="15">
+        <v>5</v>
+      </c>
+      <c r="O87" s="15">
+        <v>5</v>
+      </c>
+      <c r="P87" s="15">
+        <v>5</v>
+      </c>
+      <c r="Q87" s="15">
+        <v>5</v>
+      </c>
+      <c r="R87" s="15">
+        <v>5</v>
+      </c>
+      <c r="S87" s="15">
+        <v>5</v>
+      </c>
+      <c r="T87" s="15">
+        <v>5</v>
+      </c>
+      <c r="U87" s="15">
+        <v>5</v>
+      </c>
+      <c r="V87" s="15">
+        <v>5</v>
+      </c>
+      <c r="W87" s="15">
+        <v>5</v>
+      </c>
+      <c r="X87" s="15">
+        <v>5</v>
+      </c>
+      <c r="Y87" s="15">
+        <v>5</v>
+      </c>
+      <c r="Z87" s="15">
+        <v>5</v>
+      </c>
+      <c r="AA87" s="15">
+        <v>5</v>
+      </c>
+      <c r="AB87" s="15">
+        <v>5</v>
+      </c>
+      <c r="AC87" s="15">
+        <v>5</v>
+      </c>
+      <c r="AD87" s="15">
+        <v>5</v>
+      </c>
+      <c r="AE87" s="15">
+        <v>5</v>
+      </c>
+      <c r="AF87" s="15">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A88" s="15" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="B88" s="15">
-        <v>2020</v>
+        <v>0</v>
       </c>
       <c r="C88" s="15">
-        <v>2021</v>
+        <v>0</v>
       </c>
       <c r="D88" s="15">
-        <v>2022</v>
+        <v>0</v>
       </c>
       <c r="E88" s="15">
-        <v>2023</v>
+        <v>0</v>
       </c>
       <c r="F88" s="15">
-        <v>2024</v>
+        <v>0</v>
       </c>
       <c r="G88" s="15">
-        <v>2025</v>
+        <v>0</v>
       </c>
       <c r="H88" s="15">
-        <v>2026</v>
+        <v>0</v>
       </c>
       <c r="I88" s="15">
-        <v>2027</v>
+        <v>0</v>
       </c>
       <c r="J88" s="15">
-        <v>2028</v>
+        <v>0</v>
       </c>
       <c r="K88" s="15">
-        <v>2029</v>
+        <v>0</v>
       </c>
       <c r="L88" s="15">
-        <v>2030</v>
+        <v>0</v>
       </c>
       <c r="M88" s="15">
-        <v>2031</v>
+        <v>0</v>
       </c>
       <c r="N88" s="15">
-        <v>2032</v>
+        <v>0</v>
       </c>
       <c r="O88" s="15">
-        <v>2033</v>
+        <v>0</v>
       </c>
       <c r="P88" s="15">
-        <v>2034</v>
+        <v>0</v>
       </c>
       <c r="Q88" s="15">
-        <v>2035</v>
+        <v>0</v>
       </c>
       <c r="R88" s="15">
-        <v>2036</v>
+        <v>0</v>
       </c>
       <c r="S88" s="15">
-        <v>2037</v>
+        <v>0</v>
       </c>
       <c r="T88" s="15">
-        <v>2038</v>
+        <v>0</v>
       </c>
       <c r="U88" s="15">
-        <v>2039</v>
+        <v>0</v>
       </c>
       <c r="V88" s="15">
-        <v>2040</v>
+        <v>0</v>
       </c>
       <c r="W88" s="15">
-        <v>2041</v>
+        <v>0</v>
       </c>
       <c r="X88" s="15">
-        <v>2042</v>
+        <v>0</v>
       </c>
       <c r="Y88" s="15">
-        <v>2043</v>
+        <v>0</v>
       </c>
       <c r="Z88" s="15">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="AA88" s="15">
-        <v>2045</v>
+        <v>0</v>
       </c>
       <c r="AB88" s="15">
-        <v>2046</v>
+        <v>0</v>
       </c>
       <c r="AC88" s="15">
-        <v>2047</v>
+        <v>0</v>
       </c>
       <c r="AD88" s="15">
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="AE88" s="15">
-        <v>2049</v>
+        <v>0</v>
       </c>
       <c r="AF88" s="15">
-        <v>2050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A89" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" s="15">
+        <v>0</v>
+      </c>
+      <c r="C89" s="15">
+        <v>0</v>
+      </c>
+      <c r="D89" s="15">
+        <v>0</v>
+      </c>
+      <c r="E89" s="15">
+        <v>0</v>
+      </c>
+      <c r="F89" s="15">
+        <v>0</v>
+      </c>
+      <c r="G89" s="15">
+        <v>0</v>
+      </c>
+      <c r="H89" s="15">
+        <v>0</v>
+      </c>
+      <c r="I89" s="15">
+        <v>0</v>
+      </c>
+      <c r="J89" s="15">
+        <v>0</v>
+      </c>
+      <c r="K89" s="15">
+        <v>0</v>
+      </c>
+      <c r="L89" s="15">
+        <v>0</v>
+      </c>
+      <c r="M89" s="15">
+        <v>0</v>
+      </c>
+      <c r="N89" s="15">
+        <v>0</v>
+      </c>
+      <c r="O89" s="15">
+        <v>0</v>
+      </c>
+      <c r="P89" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="15">
+        <v>0</v>
+      </c>
+      <c r="R89" s="15">
+        <v>0</v>
+      </c>
+      <c r="S89" s="15">
+        <v>0</v>
+      </c>
+      <c r="T89" s="15">
+        <v>0</v>
+      </c>
+      <c r="U89" s="15">
+        <v>0</v>
+      </c>
+      <c r="V89" s="15">
+        <v>0</v>
+      </c>
+      <c r="W89" s="15">
+        <v>0</v>
+      </c>
+      <c r="X89" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y89" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z89" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC89" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD89" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE89" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF89" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A90" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" s="15">
+        <v>2.16E-3</v>
+      </c>
+      <c r="C90" s="15">
+        <v>2.3154429999999999E-3</v>
+      </c>
+      <c r="D90" s="15">
+        <v>3.8036620000000002E-3</v>
+      </c>
+      <c r="E90" s="15">
+        <v>5.3024580000000003E-3</v>
+      </c>
+      <c r="F90" s="15">
+        <v>6.8161840000000003E-3</v>
+      </c>
+      <c r="G90" s="15">
+        <v>8.3520650000000005E-3</v>
+      </c>
+      <c r="H90" s="15">
+        <v>9.9196909999999996E-3</v>
+      </c>
+      <c r="I90" s="15">
+        <v>1.1533804E-2</v>
+      </c>
+      <c r="J90" s="15">
+        <v>1.3212750000000001E-2</v>
+      </c>
+      <c r="K90" s="15">
+        <v>1.4978709E-2</v>
+      </c>
+      <c r="L90" s="15">
+        <v>1.6867157000000001E-2</v>
+      </c>
+      <c r="M90" s="15">
+        <v>1.7452430000000001E-2</v>
+      </c>
+      <c r="N90" s="15">
+        <v>1.8252092000000001E-2</v>
+      </c>
+      <c r="O90" s="15">
+        <v>1.9309627999999999E-2</v>
+      </c>
+      <c r="P90" s="15">
+        <v>2.0645547E-2</v>
+      </c>
+      <c r="Q90" s="15">
+        <v>2.227985E-2</v>
+      </c>
+      <c r="R90" s="15">
+        <v>2.4351382000000001E-2</v>
+      </c>
+      <c r="S90" s="15">
+        <v>2.6780347999999999E-2</v>
+      </c>
+      <c r="T90" s="15">
+        <v>2.9592798E-2</v>
+      </c>
+      <c r="U90" s="15">
+        <v>3.2960165999999999E-2</v>
+      </c>
+      <c r="V90" s="15">
+        <v>3.7044072999999997E-2</v>
+      </c>
+      <c r="W90" s="15">
+        <v>4.2587001999999999E-2</v>
+      </c>
+      <c r="X90" s="15">
+        <v>4.8824688999999998E-2</v>
+      </c>
+      <c r="Y90" s="15">
+        <v>5.5696411000000001E-2</v>
+      </c>
+      <c r="Z90" s="15">
+        <v>6.2507718000000004E-2</v>
+      </c>
+      <c r="AA90" s="15">
+        <v>6.8291605000000005E-2</v>
+      </c>
+      <c r="AB90" s="15">
+        <v>7.2692810999999996E-2</v>
+      </c>
+      <c r="AC90" s="15">
+        <v>7.5988175000000005E-2</v>
+      </c>
+      <c r="AD90" s="15">
+        <v>7.8326194000000002E-2</v>
+      </c>
+      <c r="AE90" s="15">
+        <v>8.0239419000000006E-2</v>
+      </c>
+      <c r="AF90" s="15">
+        <v>8.1928860000000006E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A92" s="15" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="93" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A93" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B93" s="15">
+        <v>2020</v>
+      </c>
+      <c r="C93" s="15">
+        <v>2021</v>
+      </c>
+      <c r="D93" s="15">
+        <v>2022</v>
+      </c>
+      <c r="E93" s="15">
+        <v>2023</v>
+      </c>
+      <c r="F93" s="15">
+        <v>2024</v>
+      </c>
+      <c r="G93" s="15">
+        <v>2025</v>
+      </c>
+      <c r="H93" s="15">
+        <v>2026</v>
+      </c>
+      <c r="I93" s="15">
+        <v>2027</v>
+      </c>
+      <c r="J93" s="15">
+        <v>2028</v>
+      </c>
+      <c r="K93" s="15">
+        <v>2029</v>
+      </c>
+      <c r="L93" s="15">
+        <v>2030</v>
+      </c>
+      <c r="M93" s="15">
+        <v>2031</v>
+      </c>
+      <c r="N93" s="15">
+        <v>2032</v>
+      </c>
+      <c r="O93" s="15">
+        <v>2033</v>
+      </c>
+      <c r="P93" s="15">
+        <v>2034</v>
+      </c>
+      <c r="Q93" s="15">
+        <v>2035</v>
+      </c>
+      <c r="R93" s="15">
+        <v>2036</v>
+      </c>
+      <c r="S93" s="15">
+        <v>2037</v>
+      </c>
+      <c r="T93" s="15">
+        <v>2038</v>
+      </c>
+      <c r="U93" s="15">
+        <v>2039</v>
+      </c>
+      <c r="V93" s="15">
+        <v>2040</v>
+      </c>
+      <c r="W93" s="15">
+        <v>2041</v>
+      </c>
+      <c r="X93" s="15">
+        <v>2042</v>
+      </c>
+      <c r="Y93" s="15">
+        <v>2043</v>
+      </c>
+      <c r="Z93" s="15">
+        <v>2044</v>
+      </c>
+      <c r="AA93" s="15">
+        <v>2045</v>
+      </c>
+      <c r="AB93" s="15">
+        <v>2046</v>
+      </c>
+      <c r="AC93" s="15">
+        <v>2047</v>
+      </c>
+      <c r="AD93" s="15">
+        <v>2048</v>
+      </c>
+      <c r="AE93" s="15">
+        <v>2049</v>
+      </c>
+      <c r="AF93" s="15">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="94" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A94" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B89" s="15">
+      <c r="B94" s="15">
         <v>3.8708444000000002E-2</v>
       </c>
-      <c r="C89" s="15">
+      <c r="C94" s="15">
         <v>4.6440683000000003E-2</v>
       </c>
-      <c r="D89" s="15">
+      <c r="D94" s="15">
         <v>5.4172921999999998E-2</v>
       </c>
-      <c r="E89" s="15">
+      <c r="E94" s="15">
         <v>6.1905160000000001E-2</v>
       </c>
-      <c r="F89" s="15">
+      <c r="F94" s="15">
         <v>6.9637399000000003E-2</v>
       </c>
-      <c r="G89" s="15">
+      <c r="G94" s="15">
         <v>7.7369637000000005E-2</v>
       </c>
-      <c r="H89" s="15">
+      <c r="H94" s="15">
         <v>8.5101876000000007E-2</v>
       </c>
-      <c r="I89" s="15">
+      <c r="I94" s="15">
         <v>9.2834114999999995E-2</v>
       </c>
-      <c r="J89" s="15">
+      <c r="J94" s="15">
         <v>0.100566353</v>
       </c>
-      <c r="K89" s="15">
+      <c r="K94" s="15">
         <v>0.108298592</v>
       </c>
-      <c r="L89" s="15">
+      <c r="L94" s="15">
         <v>0.11603083</v>
       </c>
-      <c r="M89" s="15">
+      <c r="M94" s="15">
         <v>0.123763069</v>
       </c>
-      <c r="N89" s="15">
+      <c r="N94" s="15">
         <v>0.13149530700000001</v>
       </c>
-      <c r="O89" s="15">
+      <c r="O94" s="15">
         <v>0.13922754600000001</v>
       </c>
-      <c r="P89" s="15">
+      <c r="P94" s="15">
         <v>0.14695978500000001</v>
       </c>
-      <c r="Q89" s="15">
+      <c r="Q94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="R89" s="15">
+      <c r="R94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="S89" s="15">
+      <c r="S94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="T89" s="15">
+      <c r="T94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="U89" s="15">
+      <c r="U94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="V89" s="15">
+      <c r="V94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="W89" s="15">
+      <c r="W94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="X89" s="15">
+      <c r="X94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="Y89" s="15">
+      <c r="Y94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="Z89" s="15">
+      <c r="Z94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="AA89" s="15">
+      <c r="AA94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="AB89" s="15">
+      <c r="AB94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="AC89" s="15">
+      <c r="AC94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="AD89" s="15">
+      <c r="AD94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="AE89" s="15">
+      <c r="AE94" s="15">
         <v>0.16242426200000001</v>
       </c>
-      <c r="AF89" s="15">
+      <c r="AF94" s="15">
         <v>0.16242426200000001</v>
       </c>
     </row>

</xml_diff>